<commit_message>
0.1.14 PCB sent to production
added SMD connector and PCB redrawn
</commit_message>
<xml_diff>
--- a/Project Outputs for dv_power/BOM/dv_power.xlsx
+++ b/Project Outputs for dv_power/BOM/dv_power.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="17910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="16950"/>
   </bookViews>
   <sheets>
     <sheet name="dv_power" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Designator</t>
   </si>
@@ -53,6 +53,12 @@
     <t>PLD2-20</t>
   </si>
   <si>
+    <t>X1, X3</t>
+  </si>
+  <si>
+    <t>PLD-20</t>
+  </si>
+  <si>
     <t>VT1, VT2</t>
   </si>
   <si>
@@ -77,22 +83,19 @@
     <t>DC-DC преобразователь</t>
   </si>
   <si>
-    <t>R2, R4</t>
+    <t>СМПВ 1.5 5.0 ОВ</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4</t>
   </si>
   <si>
     <t>SMD-резистор</t>
   </si>
   <si>
-    <t>Резистор</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R1, R3</t>
-  </si>
-  <si>
-    <t>2k</t>
+    <t>ОСМ Р1-12</t>
+  </si>
+  <si>
+    <t>1к</t>
   </si>
   <si>
     <t>FU1, FU2, FU3, FU4</t>
@@ -113,7 +116,7 @@
     <t>Поляризованный SMD-конденсатор</t>
   </si>
   <si>
-    <t>Поляризованный конденсатор</t>
+    <t xml:space="preserve">ОС К53-68 </t>
   </si>
   <si>
     <t>10мкФх50В</t>
@@ -125,7 +128,7 @@
     <t>SMD-конденсатор</t>
   </si>
   <si>
-    <t>Конденсатор</t>
+    <t>К10-79</t>
   </si>
   <si>
     <t>0,1мкФ</t>
@@ -531,10 +534,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -543,13 +546,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -558,12 +561,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4"/>
       <c r="D5" s="4">
         <v>2</v>
       </c>
@@ -582,76 +587,74 @@
       <c r="D6" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4">
         <v>4</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.1.17 Finished firsion with bipolar supply
</commit_message>
<xml_diff>
--- a/Project Outputs for dv_power/BOM/dv_power.xlsx
+++ b/Project Outputs for dv_power/BOM/dv_power.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\YandexDisk2\YandexDisk\OAI_NSU\Altium_projects\KVV\dv_power\Project Outputs for dv_power\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelemeshko-OAI\YandexDisk\OAI_NSU\Altium_projects\KVV\dv_power\Project Outputs for dv_power\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="16950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14265"/>
   </bookViews>
   <sheets>
     <sheet name="dv_power" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">dv_power!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Designator</t>
   </si>
@@ -59,15 +59,6 @@
     <t>PLD-20</t>
   </si>
   <si>
-    <t>VT1, VT2</t>
-  </si>
-  <si>
-    <t>Биполярный транзистор</t>
-  </si>
-  <si>
-    <t>2Т3117А/ПК "ОСМ"</t>
-  </si>
-  <si>
     <t>VD1, VD2</t>
   </si>
   <si>
@@ -86,18 +77,6 @@
     <t>СМПВ 1.5 5.0 ОВ</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4</t>
-  </si>
-  <si>
-    <t>SMD-резистор</t>
-  </si>
-  <si>
-    <t>ОСМ Р1-12</t>
-  </si>
-  <si>
-    <t>1к</t>
-  </si>
-  <si>
     <t>FU1, FU2, FU3, FU4</t>
   </si>
   <si>
@@ -110,25 +89,31 @@
     <t>0.25A</t>
   </si>
   <si>
-    <t>C2, C4, C6, C8</t>
+    <t>C8, C16</t>
+  </si>
+  <si>
+    <t>SMD-конденсатор</t>
+  </si>
+  <si>
+    <t>К10-79</t>
+  </si>
+  <si>
+    <t>10 нФ</t>
+  </si>
+  <si>
+    <t>C2, C5, C7, C10, C13, C15</t>
   </si>
   <si>
     <t>Поляризованный SMD-конденсатор</t>
   </si>
   <si>
-    <t xml:space="preserve">ОС К53-68 </t>
+    <t>ОС К53-68</t>
   </si>
   <si>
     <t>10мкФх50В</t>
   </si>
   <si>
-    <t>C1, C3, C5, C7</t>
-  </si>
-  <si>
-    <t>SMD-конденсатор</t>
-  </si>
-  <si>
-    <t>К10-79</t>
+    <t>C1, C4, C6, C9, C12, C14</t>
   </si>
   <si>
     <t>0,1мкФ</t>
@@ -191,16 +176,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -481,10 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -497,169 +473,153 @@
     <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="4">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="4">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="4">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.1.18 Version with bipolar supply
</commit_message>
<xml_diff>
--- a/Project Outputs for dv_power/BOM/dv_power.xlsx
+++ b/Project Outputs for dv_power/BOM/dv_power.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26115" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="dv_power" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">dv_power!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>